<commit_message>
Nya saker, excel och rikitga databaser
</commit_message>
<xml_diff>
--- a/site/Bok1.xlsx
+++ b/site/Bok1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>Users</t>
   </si>
@@ -84,6 +84,42 @@
   </si>
   <si>
     <t>Pucharses</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>int(2)</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>ticket</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Prod</t>
   </si>
 </sst>
 </file>
@@ -149,6 +185,13 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -156,15 +199,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,33 +528,52 @@
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="6"/>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -529,44 +584,98 @@
         <v>6</v>
       </c>
       <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="7"/>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -574,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -582,7 +691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -590,36 +699,75 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
+    <mergeCell ref="K1:N1"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="A1:D1"/>
@@ -627,6 +775,10 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="K5:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Start, loginscreen, phps, register, logedinscreen, sounds, jaokporr
</commit_message>
<xml_diff>
--- a/site/Bok1.xlsx
+++ b/site/Bok1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Users</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Prod</t>
+  </si>
+  <si>
+    <t>Foreign Key</t>
+  </si>
+  <si>
+    <t>USER_ID</t>
+  </si>
+  <si>
+    <t>Foreign key</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,6 +691,12 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -750,6 +765,12 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
       <c r="F15" t="s">
         <v>24</v>
       </c>

</xml_diff>